<commit_message>
Added pushbutton for mcu reset
</commit_message>
<xml_diff>
--- a/Bill of Materials.xlsx
+++ b/Bill of Materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Engineering Projects\Embedded Sensor Interface with FreeRTOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E22B4EB-5F2F-438C-BAED-ABCC4AD1D5E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C77C1C-DA94-47A8-B239-540BA09EBC94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="250">
   <si>
     <t>Qty</t>
   </si>
@@ -842,6 +842,15 @@
   </si>
   <si>
     <t>MCP9700T-E/TT</t>
+  </si>
+  <si>
+    <t>Switching Regulator</t>
+  </si>
+  <si>
+    <t>Tactile Switch</t>
+  </si>
+  <si>
+    <t>222AMVBAR</t>
   </si>
 </sst>
 </file>
@@ -1632,7 +1641,7 @@
   <dimension ref="A1:V102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1785,7 +1794,7 @@
         <v>237</v>
       </c>
       <c r="C4" s="36">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D4" s="34" t="s">
         <v>243</v>
@@ -1809,14 +1818,14 @@
       </c>
       <c r="L4" s="38">
         <f t="shared" ref="L4:L32" si="0">IF(C4*$L$1=0, "", C4*$L$1)</f>
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="M4" s="39">
         <v>0.62</v>
       </c>
       <c r="N4" s="40">
         <f t="shared" ref="N4:N32" si="1">IF(C4 * M4 = 0, "", C4 * M4)</f>
-        <v>3.1</v>
+        <v>3.7199999999999998</v>
       </c>
       <c r="S4" s="3" t="s">
         <v>22</v>
@@ -2047,7 +2056,9 @@
       <c r="A9" s="34">
         <v>7</v>
       </c>
-      <c r="B9" s="35"/>
+      <c r="B9" s="35" t="s">
+        <v>247</v>
+      </c>
       <c r="C9" s="36"/>
       <c r="D9" s="34"/>
       <c r="E9" s="34"/>
@@ -2083,19 +2094,29 @@
       <c r="A10" s="34">
         <v>8</v>
       </c>
-      <c r="B10" s="35"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
+      <c r="B10" s="35" t="s">
+        <v>248</v>
+      </c>
+      <c r="C10" s="36">
+        <v>2</v>
+      </c>
+      <c r="D10" s="34" t="s">
+        <v>249</v>
+      </c>
+      <c r="E10" s="34" t="s">
+        <v>19</v>
+      </c>
       <c r="F10" s="34"/>
       <c r="G10" s="34"/>
       <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
+      <c r="I10" s="34" t="s">
+        <v>178</v>
+      </c>
       <c r="J10" s="34"/>
       <c r="K10" s="37"/>
-      <c r="L10" s="38" t="str">
+      <c r="L10" s="38">
         <f t="shared" si="0"/>
-        <v/>
+        <v>2000</v>
       </c>
       <c r="M10" s="39"/>
       <c r="N10" s="40" t="str">
@@ -2954,7 +2975,7 @@
       <c r="N34" s="18">
         <f>SUM(BOM[$ Part
 Total])</f>
-        <v>9.0100000000000016</v>
+        <v>9.6300000000000008</v>
       </c>
       <c r="S34" s="3" t="s">
         <v>122</v>

</xml_diff>

<commit_message>
Added USB C receptacle components
</commit_message>
<xml_diff>
--- a/Bill of Materials.xlsx
+++ b/Bill of Materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Engineering Projects\Embedded Sensor Interface with FreeRTOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C77C1C-DA94-47A8-B239-540BA09EBC94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D734E19-57DE-4D3E-81F1-F467A27ADA50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="255">
   <si>
     <t>Qty</t>
   </si>
@@ -851,6 +851,21 @@
   </si>
   <si>
     <t>222AMVBAR</t>
+  </si>
+  <si>
+    <t>USB C Recepticle</t>
+  </si>
+  <si>
+    <t>USB4105-GF-A</t>
+  </si>
+  <si>
+    <t>5.1k Resistor</t>
+  </si>
+  <si>
+    <t>5.1k</t>
+  </si>
+  <si>
+    <t>RC0603FR-075K1L</t>
   </si>
 </sst>
 </file>
@@ -1641,7 +1656,7 @@
   <dimension ref="A1:V102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2140,24 +2155,34 @@
       <c r="A11" s="34">
         <v>9</v>
       </c>
-      <c r="B11" s="35"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
+      <c r="B11" s="35" t="s">
+        <v>250</v>
+      </c>
+      <c r="C11" s="36">
+        <v>1</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>251</v>
+      </c>
+      <c r="E11" s="34" t="s">
+        <v>224</v>
+      </c>
       <c r="F11" s="34"/>
       <c r="G11" s="34"/>
       <c r="H11" s="34"/>
       <c r="I11" s="34"/>
       <c r="J11" s="34"/>
       <c r="K11" s="37"/>
-      <c r="L11" s="38" t="str">
+      <c r="L11" s="38">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="M11" s="39"/>
-      <c r="N11" s="40" t="str">
+        <v>1000</v>
+      </c>
+      <c r="M11" s="39">
+        <v>0.78</v>
+      </c>
+      <c r="N11" s="40">
         <f t="shared" si="1"/>
-        <v/>
+        <v>0.78</v>
       </c>
       <c r="S11" s="3" t="s">
         <v>48</v>
@@ -2176,24 +2201,40 @@
       <c r="A12" s="34">
         <v>10</v>
       </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
+      <c r="B12" s="35" t="s">
+        <v>252</v>
+      </c>
+      <c r="C12" s="36">
+        <v>2</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>254</v>
+      </c>
+      <c r="E12" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="34" t="s">
+        <v>253</v>
+      </c>
       <c r="G12" s="34"/>
       <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
+      <c r="I12" s="34" t="s">
+        <v>27</v>
+      </c>
       <c r="J12" s="34"/>
-      <c r="K12" s="37"/>
-      <c r="L12" s="38" t="str">
+      <c r="K12" s="37" t="s">
+        <v>121</v>
+      </c>
+      <c r="L12" s="38">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="M12" s="39"/>
-      <c r="N12" s="40" t="str">
+        <v>2000</v>
+      </c>
+      <c r="M12" s="39">
+        <v>0.1</v>
+      </c>
+      <c r="N12" s="40">
         <f t="shared" si="1"/>
-        <v/>
+        <v>0.2</v>
       </c>
       <c r="S12" s="3" t="s">
         <v>52</v>
@@ -2975,7 +3016,7 @@
       <c r="N34" s="18">
         <f>SUM(BOM[$ Part
 Total])</f>
-        <v>9.6300000000000008</v>
+        <v>10.61</v>
       </c>
       <c r="S34" s="3" t="s">
         <v>122</v>

</xml_diff>

<commit_message>
Added components for a user pushbutton
</commit_message>
<xml_diff>
--- a/Bill of Materials.xlsx
+++ b/Bill of Materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Engineering Projects\Embedded Sensor Interface with FreeRTOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0161DD-E5E9-4023-8766-CD6BBECF1EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A7F205-3FAD-4A66-BC14-44A5CB7470D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="266">
   <si>
     <t>Qty</t>
   </si>
@@ -841,9 +841,6 @@
     <t>Temperature Sensor</t>
   </si>
   <si>
-    <t>MCP9700T-E/TT</t>
-  </si>
-  <si>
     <t>Tactile Switch</t>
   </si>
   <si>
@@ -890,6 +887,18 @@
   </si>
   <si>
     <t>Electrolytic</t>
+  </si>
+  <si>
+    <t>MCP9700AT-E/TT</t>
+  </si>
+  <si>
+    <t>10k Resistor</t>
+  </si>
+  <si>
+    <t>RMCF0603JT10K0</t>
+  </si>
+  <si>
+    <t>10k</t>
   </si>
 </sst>
 </file>
@@ -1690,7 +1699,7 @@
   <dimension ref="A1:V102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1724,7 +1733,7 @@
         <v>14</v>
       </c>
       <c r="L1" s="42">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M1" s="13" t="s">
         <v>15</v>
@@ -1815,7 +1824,7 @@
       </c>
       <c r="L3" s="31">
         <f>IF(C3*$L$1=0, "", C3*$L$1)</f>
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M3" s="32">
         <v>3.05</v>
@@ -1867,7 +1876,7 @@
       </c>
       <c r="L4" s="38">
         <f t="shared" ref="L4:L32" si="0">IF(C4*$L$1=0, "", C4*$L$1)</f>
-        <v>6000</v>
+        <v>6</v>
       </c>
       <c r="M4" s="39">
         <v>0.62</v>
@@ -1921,7 +1930,7 @@
       </c>
       <c r="L5" s="38">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M5" s="39">
         <v>0.28000000000000003</v>
@@ -1975,7 +1984,7 @@
       </c>
       <c r="L6" s="38">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M6" s="39">
         <v>0.54</v>
@@ -2029,7 +2038,7 @@
       </c>
       <c r="L7" s="38">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>2</v>
       </c>
       <c r="M7" s="39">
         <v>0.82</v>
@@ -2056,13 +2065,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C8" s="36">
         <v>2</v>
       </c>
       <c r="D8" s="44" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E8" s="34" t="s">
         <v>19</v>
@@ -2077,7 +2086,7 @@
       <c r="K8" s="37"/>
       <c r="L8" s="38">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>2</v>
       </c>
       <c r="M8" s="39">
         <v>0.22</v>
@@ -2110,7 +2119,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="44" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E9" s="34" t="s">
         <v>111</v>
@@ -2122,14 +2131,14 @@
         <v>195</v>
       </c>
       <c r="J9" s="34" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K9" s="37" t="s">
         <v>133</v>
       </c>
       <c r="L9" s="38">
         <f>IF(C9*$L$1=0, "", C9*$L$1)</f>
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M9" s="39">
         <v>0.3</v>
@@ -2156,13 +2165,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="35" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C10" s="36">
         <v>1</v>
       </c>
       <c r="D10" s="44" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E10" s="34" t="s">
         <v>30</v>
@@ -2183,7 +2192,7 @@
       </c>
       <c r="L10" s="38">
         <f>IF(C10*$L$1=0, "", C10*$L$1)</f>
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M10" s="39">
         <v>0.2</v>
@@ -2210,13 +2219,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="35" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C11" s="36">
         <v>1</v>
       </c>
       <c r="D11" s="45" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E11" s="34" t="s">
         <v>26</v>
@@ -2232,12 +2241,12 @@
         <v>20</v>
       </c>
       <c r="J11" s="34" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K11" s="37"/>
       <c r="L11" s="38">
         <f>IF(C11*$L$1=0, "", C11*$L$1)</f>
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="M11" s="39">
         <v>0.2</v>
@@ -2264,13 +2273,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="35" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C12" s="36">
         <v>2</v>
       </c>
       <c r="D12" s="45" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E12" s="34" t="s">
         <v>26</v>
@@ -2286,12 +2295,12 @@
         <v>20</v>
       </c>
       <c r="J12" s="34" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K12" s="37"/>
       <c r="L12" s="38">
         <f>IF(C12*$L$1=0, "", C12*$L$1)</f>
-        <v>2000</v>
+        <v>2</v>
       </c>
       <c r="M12" s="39">
         <v>0.91</v>
@@ -2317,24 +2326,34 @@
       <c r="A13" s="34">
         <v>11</v>
       </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="34"/>
+      <c r="B13" s="35" t="s">
+        <v>248</v>
+      </c>
+      <c r="C13" s="36">
+        <v>1</v>
+      </c>
+      <c r="D13" s="44" t="s">
+        <v>249</v>
+      </c>
+      <c r="E13" s="34" t="s">
+        <v>224</v>
+      </c>
       <c r="F13" s="34"/>
       <c r="G13" s="34"/>
       <c r="H13" s="34"/>
       <c r="I13" s="34"/>
       <c r="J13" s="34"/>
       <c r="K13" s="37"/>
-      <c r="L13" s="38" t="str">
+      <c r="L13" s="38">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="M13" s="39"/>
-      <c r="N13" s="40" t="str">
+        <v>1</v>
+      </c>
+      <c r="M13" s="39">
+        <v>0.78</v>
+      </c>
+      <c r="N13" s="40">
         <f t="shared" si="1"/>
-        <v/>
+        <v>0.78</v>
       </c>
       <c r="S13" s="3" t="s">
         <v>56</v>
@@ -2353,24 +2372,38 @@
       <c r="A14" s="34">
         <v>12</v>
       </c>
-      <c r="B14" s="35"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
+      <c r="B14" s="35" t="s">
+        <v>250</v>
+      </c>
+      <c r="C14" s="36">
+        <v>2</v>
+      </c>
+      <c r="D14" s="44" t="s">
+        <v>252</v>
+      </c>
+      <c r="E14" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="34" t="s">
+        <v>251</v>
+      </c>
       <c r="G14" s="34"/>
       <c r="H14" s="34"/>
       <c r="I14" s="34"/>
       <c r="J14" s="34"/>
-      <c r="K14" s="37"/>
-      <c r="L14" s="38" t="str">
+      <c r="K14" s="37" t="s">
+        <v>121</v>
+      </c>
+      <c r="L14" s="38">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="M14" s="39"/>
-      <c r="N14" s="40" t="str">
+        <v>2</v>
+      </c>
+      <c r="M14" s="39">
+        <v>0.1</v>
+      </c>
+      <c r="N14" s="40">
         <f t="shared" si="1"/>
-        <v/>
+        <v>0.2</v>
       </c>
       <c r="S14" s="3" t="s">
         <v>59</v>
@@ -2389,24 +2422,36 @@
       <c r="A15" s="34">
         <v>13</v>
       </c>
-      <c r="B15" s="35"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="34"/>
+      <c r="B15" s="35" t="s">
+        <v>245</v>
+      </c>
+      <c r="C15" s="36">
+        <v>1</v>
+      </c>
+      <c r="D15" s="44" t="s">
+        <v>262</v>
+      </c>
+      <c r="E15" s="34" t="s">
+        <v>114</v>
+      </c>
       <c r="F15" s="34"/>
       <c r="G15" s="34"/>
       <c r="H15" s="34"/>
       <c r="I15" s="34"/>
       <c r="J15" s="34"/>
-      <c r="K15" s="37"/>
-      <c r="L15" s="38" t="str">
+      <c r="K15" s="37" t="s">
+        <v>133</v>
+      </c>
+      <c r="L15" s="38">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="M15" s="39"/>
-      <c r="N15" s="40" t="str">
+        <v>1</v>
+      </c>
+      <c r="M15" s="39">
+        <v>0.48</v>
+      </c>
+      <c r="N15" s="40">
         <f t="shared" si="1"/>
-        <v/>
+        <v>0.48</v>
       </c>
       <c r="S15" s="3" t="s">
         <v>63</v>
@@ -2425,24 +2470,38 @@
       <c r="A16" s="34">
         <v>14</v>
       </c>
-      <c r="B16" s="35"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
+      <c r="B16" s="35" t="s">
+        <v>263</v>
+      </c>
+      <c r="C16" s="36">
+        <v>1</v>
+      </c>
+      <c r="D16" s="44" t="s">
+        <v>264</v>
+      </c>
+      <c r="E16" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="34" t="s">
+        <v>265</v>
+      </c>
       <c r="G16" s="34"/>
       <c r="H16" s="34"/>
       <c r="I16" s="34"/>
       <c r="J16" s="34"/>
-      <c r="K16" s="37"/>
-      <c r="L16" s="38" t="str">
+      <c r="K16" s="37" t="s">
+        <v>121</v>
+      </c>
+      <c r="L16" s="38">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="M16" s="39"/>
-      <c r="N16" s="40" t="str">
+        <v>1</v>
+      </c>
+      <c r="M16" s="39">
+        <v>0.1</v>
+      </c>
+      <c r="N16" s="40">
         <f t="shared" si="1"/>
-        <v/>
+        <v>0.1</v>
       </c>
       <c r="S16" s="3" t="s">
         <v>67</v>
@@ -2857,34 +2916,24 @@
       <c r="A28" s="34">
         <v>26</v>
       </c>
-      <c r="B28" s="35" t="s">
-        <v>249</v>
-      </c>
-      <c r="C28" s="36">
-        <v>1</v>
-      </c>
-      <c r="D28" s="44" t="s">
-        <v>250</v>
-      </c>
-      <c r="E28" s="34" t="s">
-        <v>224</v>
-      </c>
+      <c r="B28" s="35"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="34"/>
       <c r="F28" s="34"/>
       <c r="G28" s="34"/>
       <c r="H28" s="34"/>
       <c r="I28" s="34"/>
       <c r="J28" s="34"/>
       <c r="K28" s="37"/>
-      <c r="L28" s="38">
+      <c r="L28" s="38" t="str">
         <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="M28" s="39">
-        <v>0.78</v>
-      </c>
-      <c r="N28" s="40">
+        <v/>
+      </c>
+      <c r="M28" s="39"/>
+      <c r="N28" s="40" t="str">
         <f t="shared" si="1"/>
-        <v>0.78</v>
+        <v/>
       </c>
       <c r="S28" s="3" t="s">
         <v>108</v>
@@ -2903,40 +2952,24 @@
       <c r="A29" s="34">
         <v>27</v>
       </c>
-      <c r="B29" s="35" t="s">
-        <v>251</v>
-      </c>
-      <c r="C29" s="36">
-        <v>2</v>
-      </c>
-      <c r="D29" s="44" t="s">
-        <v>253</v>
-      </c>
-      <c r="E29" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="F29" s="34" t="s">
-        <v>252</v>
-      </c>
+      <c r="B29" s="35"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
       <c r="G29" s="34"/>
       <c r="H29" s="34"/>
-      <c r="I29" s="34" t="s">
-        <v>27</v>
-      </c>
+      <c r="I29" s="34"/>
       <c r="J29" s="34"/>
-      <c r="K29" s="37" t="s">
-        <v>121</v>
-      </c>
-      <c r="L29" s="38">
+      <c r="K29" s="37"/>
+      <c r="L29" s="38" t="str">
         <f t="shared" si="0"/>
-        <v>2000</v>
-      </c>
-      <c r="M29" s="39">
-        <v>0.1</v>
-      </c>
-      <c r="N29" s="40">
+        <v/>
+      </c>
+      <c r="M29" s="39"/>
+      <c r="N29" s="40" t="str">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v/>
       </c>
       <c r="S29" s="3" t="s">
         <v>111</v>
@@ -2991,36 +3024,24 @@
       <c r="A31" s="34">
         <v>29</v>
       </c>
-      <c r="B31" s="35" t="s">
-        <v>245</v>
-      </c>
-      <c r="C31" s="36">
-        <v>1</v>
-      </c>
-      <c r="D31" s="44" t="s">
-        <v>246</v>
-      </c>
-      <c r="E31" s="34" t="s">
-        <v>114</v>
-      </c>
+      <c r="B31" s="35"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="34"/>
       <c r="F31" s="34"/>
       <c r="G31" s="34"/>
       <c r="H31" s="34"/>
       <c r="I31" s="34"/>
       <c r="J31" s="34"/>
-      <c r="K31" s="37" t="s">
-        <v>133</v>
-      </c>
-      <c r="L31" s="38">
+      <c r="K31" s="37"/>
+      <c r="L31" s="38" t="str">
         <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="M31" s="39">
-        <v>0.4</v>
-      </c>
-      <c r="N31" s="40">
+        <v/>
+      </c>
+      <c r="M31" s="39"/>
+      <c r="N31" s="40" t="str">
         <f t="shared" si="1"/>
-        <v>0.4</v>
+        <v/>
       </c>
       <c r="S31" s="3" t="s">
         <v>117</v>
@@ -3118,7 +3139,7 @@
       <c r="N34" s="18">
         <f>SUM(BOM[$ Part
 Total])</f>
-        <v>13.569999999999999</v>
+        <v>13.749999999999998</v>
       </c>
       <c r="S34" s="3" t="s">
         <v>122</v>

</xml_diff>